<commit_message>
Updated stats; added additional tuning parameters
</commit_message>
<xml_diff>
--- a/Vaccine_Workbook.xlsx
+++ b/Vaccine_Workbook.xlsx
@@ -81,30 +81,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="R4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>James Ryan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-5-day rolling average - must update to 7 days when available</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="R5" authorId="0" shapeId="0">
       <text>
         <r>
@@ -149,11 +125,35 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
+5-day rolling average - must update to 7 days when available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>James Ryan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
 Estimates for % coverage assume a linear continuation of the latest day's trend every day until June 30th. Note that vaccine distribution is likely to increase rapidly in the coming months</t>
         </r>
       </text>
     </comment>
-    <comment ref="R9" authorId="0" shapeId="0">
+    <comment ref="R10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -177,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R14" authorId="0" shapeId="0">
+    <comment ref="R15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -201,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R15" authorId="0" shapeId="0">
+    <comment ref="R16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -225,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R17" authorId="0" shapeId="0">
+    <comment ref="R19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +245,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Assumes 85% herd immunity threshold</t>
+Assumes specified percentage herd immunity threshold</t>
         </r>
       </text>
     </comment>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -265,9 +265,6 @@
     <t>Vaccine Series Completed %</t>
   </si>
   <si>
-    <t>Days Until 6/30</t>
-  </si>
-  <si>
     <t>Pop. Initiated Vaccine Schedule (Millions)</t>
   </si>
   <si>
@@ -298,24 +295,12 @@
     <t>Change in Completed %</t>
   </si>
   <si>
-    <t>Estimated % of Pop. Started by 6/30</t>
-  </si>
-  <si>
-    <t>Estimated % of Pop. Finished by 6/30</t>
-  </si>
-  <si>
     <t>Estimated Pop. Starting Schedule/Day</t>
   </si>
   <si>
     <t>Estimated Pop. Finishing Schedule/Day</t>
   </si>
   <si>
-    <t>Estimated % of Pop., Some Protection by 6/30</t>
-  </si>
-  <si>
-    <t>Estimated % of Pop., Full Protection by 6/30</t>
-  </si>
-  <si>
     <t>Total US Cases (Lagged 2 wks, 4 mo. antibodies)</t>
   </si>
   <si>
@@ -338,6 +323,27 @@
   </si>
   <si>
     <t>Estimated Date of Herd Immunity, Full Coverage</t>
+  </si>
+  <si>
+    <t>Herd Immunity Threshold (%)</t>
+  </si>
+  <si>
+    <t>Date of Risk Determination</t>
+  </si>
+  <si>
+    <t>Days Until Date</t>
+  </si>
+  <si>
+    <t>Estimated % of Pop. Started by Date</t>
+  </si>
+  <si>
+    <t>Estimated % of Pop. Finished by Date</t>
+  </si>
+  <si>
+    <t>Estimated % of Pop., Some Protection by Date</t>
+  </si>
+  <si>
+    <t>Estimated % of Pop., Full Protection by Date</t>
   </si>
 </sst>
 </file>
@@ -396,12 +402,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -415,6 +415,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD58DE9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -495,7 +501,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -785,15 +793,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="4" width="8.88671875" customWidth="1"/>
     <col min="18" max="18" width="44.21875" customWidth="1"/>
-    <col min="19" max="19" width="11.6640625" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -804,34 +812,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -845,22 +853,21 @@
         <v>6.2</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E22" si="0">328.2*(C2/100)</f>
+        <f t="shared" ref="E2:E23" si="0">328.2*(C2/100)</f>
         <v>20.348399999999998</v>
       </c>
       <c r="G2">
         <v>1.1000000000000001</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I22" si="1">328.2*(G2/100)</f>
+        <f t="shared" ref="I2:I23" si="1">328.2*(G2/100)</f>
         <v>3.6102000000000003</v>
       </c>
-      <c r="R2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="S2" s="6">
-        <f ca="1">DATE(2021,6,30)-TODAY()</f>
-        <v>135</v>
+      <c r="R2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="15">
+        <v>44377</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -882,14 +889,14 @@
         <v>21.332999999999998</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F22" si="3">E3-E2</f>
+        <f t="shared" ref="F3:F23" si="3">E3-E2</f>
         <v>0.98460000000000036</v>
       </c>
       <c r="G3">
         <v>1.2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H22" si="4">G3-G2</f>
+        <f t="shared" ref="H3:H23" si="4">G3-G2</f>
         <v>9.9999999999999867E-2</v>
       </c>
       <c r="I3">
@@ -897,7 +904,7 @@
         <v>3.9384000000000001</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J22" si="5">I3-I2</f>
+        <f t="shared" ref="J3:J23" si="5">I3-I2</f>
         <v>0.32819999999999983</v>
       </c>
       <c r="K3">
@@ -908,12 +915,12 @@
         <f t="shared" ref="L3:L4" si="7">J3/(F3+J3)</f>
         <v>0.24999999999999983</v>
       </c>
-      <c r="R3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="S3" s="6">
-        <f ca="1">OFFSET(B1,COUNTA(B:B)-1,0)</f>
-        <v>1.64</v>
+      <c r="R3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="13">
+        <f ca="1">_xlfn.DAYS(S2,TODAY())</f>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -961,12 +968,12 @@
         <f t="shared" si="7"/>
         <v>0.39999999999999875</v>
       </c>
-      <c r="R4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="S4" s="6">
-        <f ca="1">AVERAGE(OFFSET(OFFSET(F2,COUNTA(F:F)-1,0),0,0,-7,1))</f>
-        <v>0.89082857142857208</v>
+      <c r="R4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="14">
+        <f ca="1">OFFSET(B1,COUNTA(B:B)-1,0)</f>
+        <v>1.67</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -1007,19 +1014,19 @@
         <v>0.32820000000000071</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K22" si="8">F5/(F5+J5)</f>
+        <f t="shared" ref="K5:K23" si="8">F5/(F5+J5)</f>
         <v>0.7999999999999996</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L22" si="9">J5/(F5+J5)</f>
+        <f t="shared" ref="L5:L23" si="9">J5/(F5+J5)</f>
         <v>0.20000000000000043</v>
       </c>
-      <c r="R5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5" s="6">
-        <f ca="1">AVERAGE(OFFSET(OFFSET(J2,COUNTA(J:J)-1,0),0,0,-7,1))</f>
-        <v>0.70328571428571407</v>
+      <c r="R5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" s="14">
+        <f ca="1">AVERAGE(OFFSET(OFFSET(F2,COUNTA(F:F)-1,0),0,0,-7,1))</f>
+        <v>0.93771428571428572</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -1067,12 +1074,12 @@
         <f t="shared" si="9"/>
         <v>0.40000000000000097</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="R6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="6">
-        <f ca="1">((OFFSET(E2,COUNTA(E:E)-1,0))+(S4*S2))*100/328.2</f>
-        <v>36.642857142857167</v>
+      <c r="S6" s="14">
+        <f ca="1">AVERAGE(OFFSET(OFFSET(J2,COUNTA(J:J)-1,0),0,0,-7,1))</f>
+        <v>0.75017142857142871</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -1120,12 +1127,12 @@
         <f t="shared" si="9"/>
         <v>0.24999999999999983</v>
       </c>
-      <c r="R7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="S7" s="6">
-        <f ca="1">((OFFSET(I2,COUNTA(I:I)-1,0))+(S5*S2))*100/328.2</f>
-        <v>28.92857142857142</v>
+      <c r="R7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="14">
+        <f ca="1">((OFFSET(E2,COUNTA(E:E)-1,0))+(S5*S3))*100/328.2</f>
+        <v>38.285714285714285</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -1173,6 +1180,13 @@
         <f t="shared" si="9"/>
         <v>0.24999999999999933</v>
       </c>
+      <c r="R8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S8" s="14">
+        <f ca="1">((OFFSET(I2,COUNTA(I:I)-1,0))+(S6*S3))*100/328.2</f>
+        <v>30.628571428571437</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -1219,13 +1233,6 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="S9" s="10">
-        <f>26.359-7.309</f>
-        <v>19.05</v>
-      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -1272,12 +1279,12 @@
         <f t="shared" si="9"/>
         <v>0.39999999999999836</v>
       </c>
-      <c r="R10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="S10" s="10">
-        <f>0.443-0.208</f>
-        <v>0.23500000000000001</v>
+      <c r="R10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="S10" s="8">
+        <f>26.477-7.362</f>
+        <v>19.115000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -1325,12 +1332,12 @@
         <f t="shared" si="9"/>
         <v>0.500000000000002</v>
       </c>
-      <c r="R11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="S11" s="10">
-        <f>(S9-S10)/2</f>
-        <v>9.4075000000000006</v>
+      <c r="R11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S11" s="8">
+        <f>0.447-0.209</f>
+        <v>0.23800000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1378,12 +1385,12 @@
         <f t="shared" si="9"/>
         <v>0.33333333333333304</v>
       </c>
-      <c r="R12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S12" s="10">
-        <f>S11*100/328.2</f>
-        <v>2.8663924436319324</v>
+      <c r="R12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S12" s="8">
+        <f>(S10-S11)/2</f>
+        <v>9.4385000000000012</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1431,6 +1438,13 @@
         <f t="shared" si="9"/>
         <v>0.33333333333333393</v>
       </c>
+      <c r="R13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="S13" s="8">
+        <f>S12*100/328.2</f>
+        <v>2.8758379037172461</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -1477,13 +1491,6 @@
         <f t="shared" si="9"/>
         <v>0.39999999999999825</v>
       </c>
-      <c r="R14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="S14" s="8">
-        <f ca="1">S6+S12</f>
-        <v>39.509249586489098</v>
-      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -1530,12 +1537,12 @@
         <f t="shared" si="9"/>
         <v>0.33333333333333454</v>
       </c>
-      <c r="R15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="S15" s="8">
-        <f ca="1">S7+S12</f>
-        <v>31.794963872203354</v>
+      <c r="R15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="S15" s="6">
+        <f ca="1">S7+S13</f>
+        <v>41.161552189431532</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -1583,6 +1590,13 @@
         <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
+      <c r="R16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S16" s="6">
+        <f ca="1">S8+S13</f>
+        <v>33.504409332288681</v>
+      </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -1629,13 +1643,6 @@
         <f t="shared" si="9"/>
         <v>0.50000000000000044</v>
       </c>
-      <c r="R17" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="S17" s="12">
-        <f ca="1">ROUND((85-OFFSET(C1,COUNTA(C:C)-1,0))/(S4*100/328.2),0)</f>
-        <v>269</v>
-      </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -1682,12 +1689,11 @@
         <f t="shared" si="9"/>
         <v>0.3333333333333327</v>
       </c>
-      <c r="R18" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="S18" s="13">
-        <f ca="1">TODAY()+S17</f>
-        <v>44511</v>
+      <c r="R18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="S18" s="10">
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -1735,12 +1741,12 @@
         <f t="shared" si="9"/>
         <v>0.50000000000000133</v>
       </c>
-      <c r="R19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="S19" s="12">
-        <f ca="1">ROUND((85-OFFSET(G2,COUNTA(G:G)-7,0))/(S5*100/328.2),0)</f>
-        <v>381</v>
+      <c r="R19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="S19" s="10">
+        <f ca="1">ROUND((S18-OFFSET(C1,COUNTA(C:C)-1,0))/(S5*100/328.2),0)</f>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
@@ -1788,12 +1794,12 @@
         <f t="shared" si="9"/>
         <v>0.49999999999999817</v>
       </c>
-      <c r="R20" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S20" s="13">
+      <c r="R20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="S20" s="11">
         <f ca="1">TODAY()+S19</f>
-        <v>44623</v>
+        <v>44463</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
@@ -1841,6 +1847,13 @@
         <f>J21/(F21+J21)</f>
         <v>0.40000000000000041</v>
       </c>
+      <c r="R21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="S21" s="10">
+        <f ca="1">ROUND((S18-OFFSET(G2,COUNTA(G:G)-7,0))/(S6*100/328.2),0)</f>
+        <v>312</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -1887,10 +1900,58 @@
         <f t="shared" si="9"/>
         <v>0.49999999999999595</v>
       </c>
+      <c r="R22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="11">
+        <f ca="1">TODAY()+S21</f>
+        <v>44555</v>
+      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>44243</v>
+      </c>
+      <c r="B23">
+        <v>1.67</v>
+      </c>
+      <c r="C23">
+        <v>12.2</v>
+      </c>
+      <c r="D23">
+        <f>C23-C22</f>
+        <v>0.29999999999999893</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>40.040399999999998</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>0.98459999999999326</v>
+      </c>
+      <c r="G23">
+        <v>4.7</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>15.4254</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="5"/>
+        <v>0.65640000000000143</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="8"/>
+        <v>0.59999999999999787</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="9"/>
+        <v>0.40000000000000219</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated stats; added better date functionality for natural immunity estimation
</commit_message>
<xml_diff>
--- a/Vaccine_Workbook.xlsx
+++ b/Vaccine_Workbook.xlsx
@@ -161,7 +161,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>James Ryan:</t>
         </r>
@@ -170,14 +170,86 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-To estimate natural immunity, assume that natural COVID antibodies last for 4 months (estimates on the duration of natural COVID antibodies vary from 2-8 months, and the true duration is unknown). Take total number of US cases lagged by 2 weeks (expected duration of an active COVID infection) and subtract deaths over the same period. To account for cases where immunity was lost, and for past COVID infections which have been vaccinated, take half this number as an estimate of individuals who have natural immunity.</t>
+Data for natural immunity is lagged 2 weeks to account for incubation period</t>
         </r>
       </text>
     </comment>
-    <comment ref="R15" authorId="0" shapeId="0">
+    <comment ref="R11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>James Ryan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Assume duration of natural antibodies is 16 weeks (approx. 4 months)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>James Ryan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+To estimate natural immunity, assume that natural COVID antibodies last for 4 months (estimates on the duration of natural COVID antibodies vary from 2-8 months, and the true duration is unknown). Take total number of US cases lagged by 2 weeks (expected duration of an active COVID infection) and subtract deaths over the same period. To account for cases where immunity was lost, and for past COVID infections which have been vaccinated, take overlap adjustment into account for individuals who have natural immunity.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>James Ryan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Assumed proportion of overlap between individuals receiving vaccine and individuals with natural antibodies</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,34 +270,34 @@
           </rPr>
           <t xml:space="preserve">
 For both of these figures, add estimated proportion with natural immunity to estimated population undergoing vaccines</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>James Ryan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-In theory, the gap between these two percentages will decrease over time as more individuals receive their second dose following the first (we should expect the proportion with full protection to lag behind the population with some protection by ~3wks</t>
         </r>
       </text>
     </comment>
     <comment ref="R19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>James Ryan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In theory, the gap between these two percentages will decrease over time as more individuals receive their second dose following the first (we should expect the proportion with full protection to lag behind the population with some protection by ~3wks</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -254,7 +326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -301,12 +373,6 @@
     <t>Estimated Pop. Finishing Schedule/Day</t>
   </si>
   <si>
-    <t>Total US Cases (Lagged 2 wks, 4 mo. antibodies)</t>
-  </si>
-  <si>
-    <t>Total US Deaths (Lagged 2 wks, 4 mo. antibodies)</t>
-  </si>
-  <si>
     <t>Estimated Pop. w/ Natural Immunity (50% adj.)</t>
   </si>
   <si>
@@ -344,6 +410,21 @@
   </si>
   <si>
     <t>Estimated % of Pop., Full Protection by Date</t>
+  </si>
+  <si>
+    <t>Date 16 Weeks from Lagged Date</t>
+  </si>
+  <si>
+    <t>Lagged Date (2 Weeks)</t>
+  </si>
+  <si>
+    <t>Total US Cases (Lagged 2 wks, 16 wk. antibodies)</t>
+  </si>
+  <si>
+    <t>Total US Deaths (Lagged 2 wks, 16 wk. antibodies)</t>
+  </si>
+  <si>
+    <t>Overlap Adjustment (%)</t>
   </si>
 </sst>
 </file>
@@ -489,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -506,6 +587,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
@@ -853,18 +935,18 @@
         <v>6.2</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E23" si="0">328.2*(C2/100)</f>
+        <f t="shared" ref="E2:E24" si="0">328.2*(C2/100)</f>
         <v>20.348399999999998</v>
       </c>
       <c r="G2">
         <v>1.1000000000000001</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I23" si="1">328.2*(G2/100)</f>
+        <f t="shared" ref="I2:I24" si="1">328.2*(G2/100)</f>
         <v>3.6102000000000003</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="S2" s="15">
         <v>44377</v>
@@ -889,14 +971,14 @@
         <v>21.332999999999998</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F23" si="3">E3-E2</f>
+        <f t="shared" ref="F3:F24" si="3">E3-E2</f>
         <v>0.98460000000000036</v>
       </c>
       <c r="G3">
         <v>1.2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H23" si="4">G3-G2</f>
+        <f t="shared" ref="H3:H24" si="4">G3-G2</f>
         <v>9.9999999999999867E-2</v>
       </c>
       <c r="I3">
@@ -904,7 +986,7 @@
         <v>3.9384000000000001</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J23" si="5">I3-I2</f>
+        <f t="shared" ref="J3:J24" si="5">I3-I2</f>
         <v>0.32819999999999983</v>
       </c>
       <c r="K3">
@@ -916,11 +998,11 @@
         <v>0.24999999999999983</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="S3" s="13">
         <f ca="1">_xlfn.DAYS(S2,TODAY())</f>
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -973,7 +1055,7 @@
       </c>
       <c r="S4" s="14">
         <f ca="1">OFFSET(B1,COUNTA(B:B)-1,0)</f>
-        <v>1.67</v>
+        <v>1.61</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -1014,11 +1096,11 @@
         <v>0.32820000000000071</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K23" si="8">F5/(F5+J5)</f>
+        <f t="shared" ref="K5:K24" si="8">F5/(F5+J5)</f>
         <v>0.7999999999999996</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L23" si="9">J5/(F5+J5)</f>
+        <f t="shared" ref="L5:L24" si="9">J5/(F5+J5)</f>
         <v>0.20000000000000043</v>
       </c>
       <c r="R5" s="12" t="s">
@@ -1026,7 +1108,7 @@
       </c>
       <c r="S5" s="14">
         <f ca="1">AVERAGE(OFFSET(OFFSET(F2,COUNTA(F:F)-1,0),0,0,-7,1))</f>
-        <v>0.93771428571428572</v>
+        <v>0.84394285714285744</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -1079,7 +1161,7 @@
       </c>
       <c r="S6" s="14">
         <f ca="1">AVERAGE(OFFSET(OFFSET(J2,COUNTA(J:J)-1,0),0,0,-7,1))</f>
-        <v>0.75017142857142871</v>
+        <v>0.70328571428571429</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -1128,11 +1210,11 @@
         <v>0.24999999999999983</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="S7" s="14">
         <f ca="1">((OFFSET(E2,COUNTA(E:E)-1,0))+(S5*S3))*100/328.2</f>
-        <v>38.285714285714285</v>
+        <v>34.200000000000017</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -1181,11 +1263,11 @@
         <v>0.24999999999999933</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S8" s="14">
         <f ca="1">((OFFSET(I2,COUNTA(I:I)-1,0))+(S6*S3))*100/328.2</f>
-        <v>30.628571428571437</v>
+        <v>28.500000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -1280,11 +1362,11 @@
         <v>0.39999999999999836</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="S10" s="8">
-        <f>26.477-7.362</f>
-        <v>19.115000000000002</v>
+        <v>29</v>
+      </c>
+      <c r="S10" s="16">
+        <f ca="1">TODAY()-14</f>
+        <v>44230</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -1333,11 +1415,11 @@
         <v>0.500000000000002</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="S11" s="8">
-        <f>0.447-0.209</f>
-        <v>0.23800000000000002</v>
+        <v>28</v>
+      </c>
+      <c r="S11" s="16">
+        <f ca="1">S10-(7*16)</f>
+        <v>44118</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1386,11 +1468,11 @@
         <v>0.33333333333333304</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="S12" s="8">
-        <f>(S10-S11)/2</f>
-        <v>9.4385000000000012</v>
+        <f>26.597-7.978</f>
+        <v>18.619</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1439,11 +1521,11 @@
         <v>0.33333333333333393</v>
       </c>
       <c r="R13" s="7" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="S13" s="8">
-        <f>S12*100/328.2</f>
-        <v>2.8758379037172461</v>
+        <f>0.451-0.217</f>
+        <v>0.23400000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1491,6 +1573,12 @@
         <f t="shared" si="9"/>
         <v>0.39999999999999825</v>
       </c>
+      <c r="R14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="S14" s="8">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -1537,12 +1625,12 @@
         <f t="shared" si="9"/>
         <v>0.33333333333333454</v>
       </c>
-      <c r="R15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="S15" s="6">
-        <f ca="1">S7+S13</f>
-        <v>41.161552189431532</v>
+      <c r="R15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="S15" s="8">
+        <f>(S12-S13)/(100/S14)</f>
+        <v>9.192499999999999</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -1590,12 +1678,12 @@
         <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="R16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="S16" s="6">
-        <f ca="1">S8+S13</f>
-        <v>33.504409332288681</v>
+      <c r="R16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S16" s="8">
+        <f>S15*100/328.2</f>
+        <v>2.8008836075563677</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -1689,11 +1777,12 @@
         <f t="shared" si="9"/>
         <v>0.3333333333333327</v>
       </c>
-      <c r="R18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S18" s="10">
-        <v>75</v>
+      <c r="R18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="S18" s="6">
+        <f ca="1">S7+S16</f>
+        <v>37.000883607556382</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -1741,12 +1830,12 @@
         <f t="shared" si="9"/>
         <v>0.50000000000000133</v>
       </c>
-      <c r="R19" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="S19" s="10">
-        <f ca="1">ROUND((S18-OFFSET(C1,COUNTA(C:C)-1,0))/(S5*100/328.2),0)</f>
-        <v>220</v>
+      <c r="R19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S19" s="6">
+        <f ca="1">S8+S16</f>
+        <v>31.300883607556372</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
@@ -1794,13 +1883,6 @@
         <f t="shared" si="9"/>
         <v>0.49999999999999817</v>
       </c>
-      <c r="R20" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="S20" s="11">
-        <f ca="1">TODAY()+S19</f>
-        <v>44463</v>
-      </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -1848,11 +1930,10 @@
         <v>0.40000000000000041</v>
       </c>
       <c r="R21" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S21" s="10">
-        <f ca="1">ROUND((S18-OFFSET(G2,COUNTA(G:G)-7,0))/(S6*100/328.2),0)</f>
-        <v>312</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
@@ -1901,11 +1982,11 @@
         <v>0.49999999999999595</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="S22" s="11">
-        <f ca="1">TODAY()+S21</f>
-        <v>44555</v>
+        <v>17</v>
+      </c>
+      <c r="S22" s="10">
+        <f ca="1">ROUND((S21-OFFSET(C1,COUNTA(C:C)-1,0))/(S5*100/328.2),0)</f>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
@@ -1953,15 +2034,77 @@
         <f t="shared" si="9"/>
         <v>0.40000000000000219</v>
       </c>
+      <c r="R23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="S23" s="11">
+        <f ca="1">TODAY()+S22</f>
+        <v>44488</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>44244</v>
       </c>
+      <c r="B24">
+        <v>1.61</v>
+      </c>
+      <c r="C24">
+        <v>12.3</v>
+      </c>
+      <c r="D24">
+        <f>C24-C23</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>40.368600000000001</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>0.32820000000000249</v>
+      </c>
+      <c r="G24">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="4"/>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>16.081800000000001</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="5"/>
+        <v>0.65640000000000143</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="8"/>
+        <v>0.33333333333333454</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="9"/>
+        <v>0.66666666666666541</v>
+      </c>
+      <c r="R24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="S24" s="10">
+        <f ca="1">ROUND((S21-OFFSET(G2,COUNTA(G:G)-7,0))/(S6*100/328.2),0)</f>
+        <v>332</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>44245</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="S25" s="11">
+        <f ca="1">TODAY()+S24</f>
+        <v>44576</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>